<commit_message>
Add value enum validation
</commit_message>
<xml_diff>
--- a/curation/draft/package16/R16_BC_SDTM_VS.xlsx
+++ b/curation/draft/package16/R16_BC_SDTM_VS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\package16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BF4290-42C8-4484-9317-CD245E2CDB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F725082-8929-44FF-9A28-78E47E81D87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BC_VS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12000" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12000" uniqueCount="542">
   <si>
     <t>package_date</t>
   </si>
@@ -1660,10 +1660,13 @@
     <t>8336-0</t>
   </si>
   <si>
-    <t>A measure of the 2-dimensional extent of the body surface (i.e., the skin). Body surface area (BSA) can be calculated by mathematical formula or from a chart that relates height to weight. BSA is often an important factor in dosing.</t>
-  </si>
-  <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>A measure of the 2-dimensional extent of the body surface (i.e., the skin).  Body surface area (BSA) can be calculated by mathematical formula or from a chart that relates height to weight.  BSA is often an important factor in dosing.</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -2164,7 +2167,7 @@
   <dimension ref="A1:Q189"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45:I46"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4021,7 +4024,7 @@
         <v>40</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>33</v>
@@ -4071,7 +4074,7 @@
         <v>40</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>33</v>
@@ -4124,7 +4127,7 @@
         <v>40</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>33</v>
@@ -10518,7 +10521,7 @@
   <dimension ref="A1:AF473"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10656,7 +10659,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>390</v>
       </c>
@@ -10721,7 +10724,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>390</v>
       </c>
@@ -10830,7 +10833,7 @@
         <v>445</v>
       </c>
       <c r="W4" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X4" s="16">
         <v>8</v>
@@ -10969,7 +10972,7 @@
         <v>445</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X6" s="16">
         <v>8</v>
@@ -11037,7 +11040,7 @@
         <v>445</v>
       </c>
       <c r="W7" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X7" s="16">
         <v>8</v>
@@ -11350,7 +11353,7 @@
         <v>445</v>
       </c>
       <c r="W12" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X12" s="16">
         <v>8</v>
@@ -11424,7 +11427,7 @@
         <v>445</v>
       </c>
       <c r="W13" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X13" s="16">
         <v>8</v>
@@ -11492,7 +11495,7 @@
         <v>445</v>
       </c>
       <c r="W14" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X14" s="16">
         <v>8</v>
@@ -11740,7 +11743,7 @@
         <v>445</v>
       </c>
       <c r="W18" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X18" s="16">
         <v>8</v>
@@ -11879,7 +11882,7 @@
         <v>445</v>
       </c>
       <c r="W20" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X20" s="16">
         <v>8</v>
@@ -11947,7 +11950,7 @@
         <v>445</v>
       </c>
       <c r="W21" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X21" s="16">
         <v>8</v>
@@ -12260,7 +12263,7 @@
         <v>445</v>
       </c>
       <c r="W26" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X26" s="16">
         <v>8</v>
@@ -12334,7 +12337,7 @@
         <v>445</v>
       </c>
       <c r="W27" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X27" s="16">
         <v>8</v>
@@ -12402,7 +12405,7 @@
         <v>445</v>
       </c>
       <c r="W28" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X28" s="16">
         <v>8</v>
@@ -12650,7 +12653,7 @@
         <v>445</v>
       </c>
       <c r="W32" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X32" s="16">
         <v>8</v>
@@ -12789,7 +12792,7 @@
         <v>445</v>
       </c>
       <c r="W34" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X34" s="16">
         <v>8</v>
@@ -12857,7 +12860,7 @@
         <v>445</v>
       </c>
       <c r="W35" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X35" s="16">
         <v>8</v>
@@ -13170,7 +13173,7 @@
         <v>445</v>
       </c>
       <c r="W40" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X40" s="16">
         <v>8</v>
@@ -13309,7 +13312,7 @@
         <v>445</v>
       </c>
       <c r="W42" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X42" s="16">
         <v>8</v>
@@ -13377,7 +13380,7 @@
         <v>445</v>
       </c>
       <c r="W43" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X43" s="16">
         <v>8</v>
@@ -13690,7 +13693,7 @@
         <v>445</v>
       </c>
       <c r="W48" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X48" s="16">
         <v>8</v>
@@ -13829,7 +13832,7 @@
         <v>445</v>
       </c>
       <c r="W50" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X50" s="16">
         <v>8</v>
@@ -13897,7 +13900,7 @@
         <v>445</v>
       </c>
       <c r="W51" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X51" s="16">
         <v>8</v>
@@ -14210,7 +14213,7 @@
         <v>445</v>
       </c>
       <c r="W56" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X56" s="16">
         <v>8</v>
@@ -14349,7 +14352,7 @@
         <v>445</v>
       </c>
       <c r="W58" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X58" s="16">
         <v>8</v>
@@ -14417,7 +14420,7 @@
         <v>445</v>
       </c>
       <c r="W59" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X59" s="16">
         <v>8</v>
@@ -14730,7 +14733,7 @@
         <v>445</v>
       </c>
       <c r="W64" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X64" s="16">
         <v>8</v>
@@ -14804,7 +14807,7 @@
         <v>445</v>
       </c>
       <c r="W65" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X65" s="16">
         <v>8</v>
@@ -14872,7 +14875,7 @@
         <v>445</v>
       </c>
       <c r="W66" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X66" s="16">
         <v>8</v>
@@ -15120,7 +15123,7 @@
         <v>445</v>
       </c>
       <c r="W70" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X70" s="16">
         <v>8</v>
@@ -15259,7 +15262,7 @@
         <v>445</v>
       </c>
       <c r="W72" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X72" s="16">
         <v>8</v>
@@ -15327,7 +15330,7 @@
         <v>445</v>
       </c>
       <c r="W73" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X73" s="16">
         <v>8</v>
@@ -15640,7 +15643,7 @@
         <v>445</v>
       </c>
       <c r="W78" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X78" s="16">
         <v>8</v>
@@ -15779,7 +15782,7 @@
         <v>445</v>
       </c>
       <c r="W80" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X80" s="16">
         <v>8</v>
@@ -15847,7 +15850,7 @@
         <v>445</v>
       </c>
       <c r="W81" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X81" s="16">
         <v>8</v>
@@ -16160,7 +16163,7 @@
         <v>445</v>
       </c>
       <c r="W86" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X86" s="16">
         <v>8</v>
@@ -16299,7 +16302,7 @@
         <v>445</v>
       </c>
       <c r="W88" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X88" s="16">
         <v>8</v>
@@ -16367,7 +16370,7 @@
         <v>445</v>
       </c>
       <c r="W89" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X89" s="16">
         <v>8</v>
@@ -16680,7 +16683,7 @@
         <v>445</v>
       </c>
       <c r="W94" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X94" s="16">
         <v>8</v>
@@ -16819,7 +16822,7 @@
         <v>445</v>
       </c>
       <c r="W96" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X96" s="16">
         <v>8</v>
@@ -16887,7 +16890,7 @@
         <v>445</v>
       </c>
       <c r="W97" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X97" s="16">
         <v>8</v>
@@ -17200,7 +17203,7 @@
         <v>445</v>
       </c>
       <c r="W102" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X102" s="16">
         <v>8</v>
@@ -17339,7 +17342,7 @@
         <v>445</v>
       </c>
       <c r="W104" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X104" s="16">
         <v>8</v>
@@ -17407,7 +17410,7 @@
         <v>445</v>
       </c>
       <c r="W105" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X105" s="16">
         <v>8</v>
@@ -17785,7 +17788,7 @@
         <v>445</v>
       </c>
       <c r="W111" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X111" s="16">
         <v>8</v>
@@ -17924,7 +17927,7 @@
         <v>445</v>
       </c>
       <c r="W113" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X113" s="16">
         <v>8</v>
@@ -17992,7 +17995,7 @@
         <v>445</v>
       </c>
       <c r="W114" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X114" s="16">
         <v>8</v>
@@ -18305,7 +18308,7 @@
         <v>445</v>
       </c>
       <c r="W119" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X119" s="16">
         <v>8</v>
@@ -18379,7 +18382,7 @@
         <v>445</v>
       </c>
       <c r="W120" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X120" s="16">
         <v>8</v>
@@ -18447,7 +18450,7 @@
         <v>445</v>
       </c>
       <c r="W121" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X121" s="16">
         <v>8</v>
@@ -18695,7 +18698,7 @@
         <v>445</v>
       </c>
       <c r="W125" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X125" s="16">
         <v>8</v>
@@ -18769,7 +18772,7 @@
         <v>445</v>
       </c>
       <c r="W126" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X126" s="16">
         <v>8</v>
@@ -18837,7 +18840,7 @@
         <v>445</v>
       </c>
       <c r="W127" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X127" s="16">
         <v>8</v>
@@ -19085,7 +19088,7 @@
         <v>445</v>
       </c>
       <c r="W131" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X131" s="16">
         <v>8</v>
@@ -19224,7 +19227,7 @@
         <v>445</v>
       </c>
       <c r="W133" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X133" s="16">
         <v>8</v>
@@ -19292,7 +19295,7 @@
         <v>445</v>
       </c>
       <c r="W134" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X134" s="16">
         <v>8</v>
@@ -19605,7 +19608,7 @@
         <v>445</v>
       </c>
       <c r="W139" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X139" s="16">
         <v>8</v>
@@ -19744,7 +19747,7 @@
         <v>445</v>
       </c>
       <c r="W141" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X141" s="16">
         <v>8</v>
@@ -19812,7 +19815,7 @@
         <v>445</v>
       </c>
       <c r="W142" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X142" s="16">
         <v>8</v>
@@ -20125,7 +20128,7 @@
         <v>445</v>
       </c>
       <c r="W147" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X147" s="16">
         <v>8</v>
@@ -20264,7 +20267,7 @@
         <v>445</v>
       </c>
       <c r="W149" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X149" s="16">
         <v>8</v>
@@ -20332,7 +20335,7 @@
         <v>445</v>
       </c>
       <c r="W150" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X150" s="16">
         <v>8</v>
@@ -20645,7 +20648,7 @@
         <v>445</v>
       </c>
       <c r="W155" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X155" s="16">
         <v>8</v>
@@ -20784,7 +20787,7 @@
         <v>445</v>
       </c>
       <c r="W157" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X157" s="16">
         <v>8</v>
@@ -20852,7 +20855,7 @@
         <v>445</v>
       </c>
       <c r="W158" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X158" s="16">
         <v>8</v>
@@ -21165,7 +21168,7 @@
         <v>445</v>
       </c>
       <c r="W163" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X163" s="16">
         <v>8</v>
@@ -21304,7 +21307,7 @@
         <v>445</v>
       </c>
       <c r="W165" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X165" s="16">
         <v>8</v>
@@ -21372,7 +21375,7 @@
         <v>445</v>
       </c>
       <c r="W166" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X166" s="16">
         <v>8</v>
@@ -21685,7 +21688,7 @@
         <v>445</v>
       </c>
       <c r="W171" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X171" s="16">
         <v>8</v>
@@ -21824,7 +21827,7 @@
         <v>445</v>
       </c>
       <c r="W173" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X173" s="16">
         <v>8</v>
@@ -21892,7 +21895,7 @@
         <v>445</v>
       </c>
       <c r="W174" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X174" s="16">
         <v>8</v>
@@ -22205,7 +22208,7 @@
         <v>445</v>
       </c>
       <c r="W179" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X179" s="16">
         <v>8</v>
@@ -22344,7 +22347,7 @@
         <v>445</v>
       </c>
       <c r="W181" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X181" s="16">
         <v>8</v>
@@ -22412,7 +22415,7 @@
         <v>445</v>
       </c>
       <c r="W182" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X182" s="16">
         <v>8</v>
@@ -22725,7 +22728,7 @@
         <v>445</v>
       </c>
       <c r="W187" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X187" s="16">
         <v>8</v>
@@ -22864,7 +22867,7 @@
         <v>445</v>
       </c>
       <c r="W189" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X189" s="16">
         <v>8</v>
@@ -22932,7 +22935,7 @@
         <v>445</v>
       </c>
       <c r="W190" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X190" s="16">
         <v>8</v>
@@ -23245,7 +23248,7 @@
         <v>445</v>
       </c>
       <c r="W195" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X195" s="16">
         <v>8</v>
@@ -23384,7 +23387,7 @@
         <v>445</v>
       </c>
       <c r="W197" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X197" s="16">
         <v>8</v>
@@ -23452,7 +23455,7 @@
         <v>445</v>
       </c>
       <c r="W198" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X198" s="16">
         <v>8</v>
@@ -23765,7 +23768,7 @@
         <v>445</v>
       </c>
       <c r="W203" s="16" t="s">
-        <v>25</v>
+        <v>541</v>
       </c>
       <c r="X203" s="16">
         <v>20</v>
@@ -23833,7 +23836,7 @@
         <v>445</v>
       </c>
       <c r="W204" s="16" t="s">
-        <v>25</v>
+        <v>541</v>
       </c>
       <c r="X204" s="16">
         <v>20</v>
@@ -24075,7 +24078,7 @@
         <v>445</v>
       </c>
       <c r="W208" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X208" s="16">
         <v>8</v>
@@ -24149,7 +24152,7 @@
         <v>445</v>
       </c>
       <c r="W209" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X209" s="16">
         <v>8</v>
@@ -24217,7 +24220,7 @@
         <v>445</v>
       </c>
       <c r="W210" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X210" s="16">
         <v>8</v>
@@ -24465,7 +24468,7 @@
         <v>445</v>
       </c>
       <c r="W214" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X214" s="16">
         <v>8</v>
@@ -24604,7 +24607,7 @@
         <v>445</v>
       </c>
       <c r="W216" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X216" s="16">
         <v>8</v>
@@ -24672,7 +24675,7 @@
         <v>445</v>
       </c>
       <c r="W217" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X217" s="16">
         <v>8</v>
@@ -24985,7 +24988,7 @@
         <v>445</v>
       </c>
       <c r="W222" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X222" s="16">
         <v>8</v>
@@ -25124,7 +25127,7 @@
         <v>445</v>
       </c>
       <c r="W224" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X224" s="16">
         <v>8</v>
@@ -25192,7 +25195,7 @@
         <v>445</v>
       </c>
       <c r="W225" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X225" s="16">
         <v>8</v>
@@ -25505,7 +25508,7 @@
         <v>445</v>
       </c>
       <c r="W230" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X230" s="16">
         <v>8</v>
@@ -25644,7 +25647,7 @@
         <v>445</v>
       </c>
       <c r="W232" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X232" s="16">
         <v>8</v>
@@ -25712,7 +25715,7 @@
         <v>445</v>
       </c>
       <c r="W233" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X233" s="16">
         <v>8</v>
@@ -26025,7 +26028,7 @@
         <v>445</v>
       </c>
       <c r="W238" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X238" s="16">
         <v>8</v>
@@ -26099,7 +26102,7 @@
         <v>445</v>
       </c>
       <c r="W239" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X239" s="16">
         <v>8</v>
@@ -26167,7 +26170,7 @@
         <v>445</v>
       </c>
       <c r="W240" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X240" s="16">
         <v>8</v>
@@ -26415,7 +26418,7 @@
         <v>445</v>
       </c>
       <c r="W244" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X244" s="16">
         <v>8</v>
@@ -26554,7 +26557,7 @@
         <v>445</v>
       </c>
       <c r="W246" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X246" s="16">
         <v>8</v>
@@ -26622,7 +26625,7 @@
         <v>445</v>
       </c>
       <c r="W247" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X247" s="16">
         <v>8</v>
@@ -26935,7 +26938,7 @@
         <v>445</v>
       </c>
       <c r="W252" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X252" s="16">
         <v>8</v>
@@ -27074,7 +27077,7 @@
         <v>445</v>
       </c>
       <c r="W254" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X254" s="16">
         <v>8</v>
@@ -27142,7 +27145,7 @@
         <v>445</v>
       </c>
       <c r="W255" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X255" s="16">
         <v>8</v>
@@ -27455,7 +27458,7 @@
         <v>445</v>
       </c>
       <c r="W260" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X260" s="16">
         <v>8</v>
@@ -27529,7 +27532,7 @@
         <v>445</v>
       </c>
       <c r="W261" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X261" s="16">
         <v>8</v>
@@ -27597,7 +27600,7 @@
         <v>445</v>
       </c>
       <c r="W262" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X262" s="16">
         <v>8</v>
@@ -27845,7 +27848,7 @@
         <v>445</v>
       </c>
       <c r="W266" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X266" s="16">
         <v>8</v>
@@ -27984,7 +27987,7 @@
         <v>445</v>
       </c>
       <c r="W268" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X268" s="16">
         <v>8</v>
@@ -28052,7 +28055,7 @@
         <v>445</v>
       </c>
       <c r="W269" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X269" s="16">
         <v>8</v>
@@ -28365,7 +28368,7 @@
         <v>445</v>
       </c>
       <c r="W274" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X274" s="16">
         <v>8</v>
@@ -28504,7 +28507,7 @@
         <v>445</v>
       </c>
       <c r="W276" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X276" s="16">
         <v>8</v>
@@ -28572,7 +28575,7 @@
         <v>445</v>
       </c>
       <c r="W277" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X277" s="16">
         <v>8</v>
@@ -28885,7 +28888,7 @@
         <v>445</v>
       </c>
       <c r="W282" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X282" s="16">
         <v>8</v>
@@ -29024,7 +29027,7 @@
         <v>445</v>
       </c>
       <c r="W284" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X284" s="16">
         <v>8</v>
@@ -29092,7 +29095,7 @@
         <v>445</v>
       </c>
       <c r="W285" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X285" s="16">
         <v>8</v>
@@ -29405,7 +29408,7 @@
         <v>445</v>
       </c>
       <c r="W290" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X290" s="16">
         <v>8</v>
@@ -29544,7 +29547,7 @@
         <v>445</v>
       </c>
       <c r="W292" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X292" s="16">
         <v>8</v>
@@ -29612,7 +29615,7 @@
         <v>445</v>
       </c>
       <c r="W293" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X293" s="16">
         <v>8</v>
@@ -29925,7 +29928,7 @@
         <v>445</v>
       </c>
       <c r="W298" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X298" s="16">
         <v>8</v>
@@ -30064,7 +30067,7 @@
         <v>445</v>
       </c>
       <c r="W300" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X300" s="16">
         <v>8</v>
@@ -30132,7 +30135,7 @@
         <v>445</v>
       </c>
       <c r="W301" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X301" s="16">
         <v>8</v>
@@ -30445,7 +30448,7 @@
         <v>445</v>
       </c>
       <c r="W306" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X306" s="16">
         <v>8</v>
@@ -30584,7 +30587,7 @@
         <v>445</v>
       </c>
       <c r="W308" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X308" s="16">
         <v>8</v>
@@ -30652,7 +30655,7 @@
         <v>445</v>
       </c>
       <c r="W309" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X309" s="16">
         <v>8</v>
@@ -30965,7 +30968,7 @@
         <v>445</v>
       </c>
       <c r="W314" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X314" s="16">
         <v>8</v>
@@ -31104,7 +31107,7 @@
         <v>445</v>
       </c>
       <c r="W316" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X316" s="16">
         <v>8</v>
@@ -31172,7 +31175,7 @@
         <v>445</v>
       </c>
       <c r="W317" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X317" s="16">
         <v>8</v>
@@ -31485,7 +31488,7 @@
         <v>445</v>
       </c>
       <c r="W322" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X322" s="16">
         <v>8</v>
@@ -31624,7 +31627,7 @@
         <v>445</v>
       </c>
       <c r="W324" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X324" s="16">
         <v>8</v>
@@ -31692,7 +31695,7 @@
         <v>445</v>
       </c>
       <c r="W325" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X325" s="16">
         <v>8</v>
@@ -32005,7 +32008,7 @@
         <v>445</v>
       </c>
       <c r="W330" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X330" s="16">
         <v>8</v>
@@ -32144,7 +32147,7 @@
         <v>445</v>
       </c>
       <c r="W332" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X332" s="16">
         <v>8</v>
@@ -32212,7 +32215,7 @@
         <v>445</v>
       </c>
       <c r="W333" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X333" s="16">
         <v>8</v>
@@ -32525,7 +32528,7 @@
         <v>445</v>
       </c>
       <c r="W338" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X338" s="16">
         <v>8</v>
@@ -32664,7 +32667,7 @@
         <v>445</v>
       </c>
       <c r="W340" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X340" s="16">
         <v>8</v>
@@ -32732,7 +32735,7 @@
         <v>445</v>
       </c>
       <c r="W341" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X341" s="16">
         <v>8</v>
@@ -33045,7 +33048,7 @@
         <v>445</v>
       </c>
       <c r="W346" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X346" s="16">
         <v>8</v>
@@ -33184,7 +33187,7 @@
         <v>445</v>
       </c>
       <c r="W348" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X348" s="16">
         <v>8</v>
@@ -33252,7 +33255,7 @@
         <v>445</v>
       </c>
       <c r="W349" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X349" s="16">
         <v>8</v>
@@ -33565,7 +33568,7 @@
         <v>445</v>
       </c>
       <c r="W354" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X354" s="16">
         <v>8</v>
@@ -33704,7 +33707,7 @@
         <v>445</v>
       </c>
       <c r="W356" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X356" s="16">
         <v>8</v>
@@ -33772,7 +33775,7 @@
         <v>445</v>
       </c>
       <c r="W357" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X357" s="16">
         <v>8</v>
@@ -34085,7 +34088,7 @@
         <v>445</v>
       </c>
       <c r="W362" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X362" s="16">
         <v>8</v>
@@ -34224,7 +34227,7 @@
         <v>445</v>
       </c>
       <c r="W364" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X364" s="16">
         <v>8</v>
@@ -34292,7 +34295,7 @@
         <v>445</v>
       </c>
       <c r="W365" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X365" s="16">
         <v>8</v>
@@ -34670,7 +34673,7 @@
         <v>445</v>
       </c>
       <c r="W371" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X371" s="16">
         <v>8</v>
@@ -34809,7 +34812,7 @@
         <v>445</v>
       </c>
       <c r="W373" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X373" s="16">
         <v>8</v>
@@ -34877,7 +34880,7 @@
         <v>445</v>
       </c>
       <c r="W374" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X374" s="16">
         <v>8</v>
@@ -35255,7 +35258,7 @@
         <v>445</v>
       </c>
       <c r="W380" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X380" s="16">
         <v>8</v>
@@ -35394,7 +35397,7 @@
         <v>445</v>
       </c>
       <c r="W382" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X382" s="16">
         <v>8</v>
@@ -35462,7 +35465,7 @@
         <v>445</v>
       </c>
       <c r="W383" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X383" s="16">
         <v>8</v>
@@ -35775,7 +35778,7 @@
         <v>445</v>
       </c>
       <c r="W388" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X388" s="16">
         <v>8</v>
@@ -35914,7 +35917,7 @@
         <v>445</v>
       </c>
       <c r="W390" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X390" s="16">
         <v>8</v>
@@ -35982,7 +35985,7 @@
         <v>445</v>
       </c>
       <c r="W391" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X391" s="16">
         <v>8</v>
@@ -36295,7 +36298,7 @@
         <v>445</v>
       </c>
       <c r="W396" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X396" s="16">
         <v>8</v>
@@ -36369,7 +36372,7 @@
         <v>445</v>
       </c>
       <c r="W397" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X397" s="16">
         <v>8</v>
@@ -36437,7 +36440,7 @@
         <v>445</v>
       </c>
       <c r="W398" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X398" s="16">
         <v>8</v>
@@ -36685,7 +36688,7 @@
         <v>445</v>
       </c>
       <c r="W402" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X402" s="16">
         <v>8</v>
@@ -36759,7 +36762,7 @@
         <v>445</v>
       </c>
       <c r="W403" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X403" s="16">
         <v>8</v>
@@ -36827,7 +36830,7 @@
         <v>445</v>
       </c>
       <c r="W404" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X404" s="16">
         <v>8</v>
@@ -37075,7 +37078,7 @@
         <v>445</v>
       </c>
       <c r="W408" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X408" s="16">
         <v>8</v>
@@ -37214,7 +37217,7 @@
         <v>445</v>
       </c>
       <c r="W410" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X410" s="16">
         <v>8</v>
@@ -37282,7 +37285,7 @@
         <v>445</v>
       </c>
       <c r="W411" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X411" s="16">
         <v>8</v>
@@ -37595,7 +37598,7 @@
         <v>445</v>
       </c>
       <c r="W416" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X416" s="16">
         <v>8</v>
@@ -37734,7 +37737,7 @@
         <v>445</v>
       </c>
       <c r="W418" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X418" s="16">
         <v>8</v>
@@ -37802,7 +37805,7 @@
         <v>445</v>
       </c>
       <c r="W419" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X419" s="16">
         <v>8</v>
@@ -38115,7 +38118,7 @@
         <v>445</v>
       </c>
       <c r="W424" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X424" s="16">
         <v>8</v>
@@ -38254,7 +38257,7 @@
         <v>445</v>
       </c>
       <c r="W426" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X426" s="16">
         <v>8</v>
@@ -38322,7 +38325,7 @@
         <v>445</v>
       </c>
       <c r="W427" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X427" s="16">
         <v>8</v>
@@ -38635,7 +38638,7 @@
         <v>445</v>
       </c>
       <c r="W432" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X432" s="16">
         <v>8</v>
@@ -38774,7 +38777,7 @@
         <v>445</v>
       </c>
       <c r="W434" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X434" s="16">
         <v>8</v>
@@ -38842,7 +38845,7 @@
         <v>445</v>
       </c>
       <c r="W435" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X435" s="16">
         <v>8</v>
@@ -39155,7 +39158,7 @@
         <v>445</v>
       </c>
       <c r="W440" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X440" s="16">
         <v>8</v>
@@ -39294,7 +39297,7 @@
         <v>445</v>
       </c>
       <c r="W442" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X442" s="16">
         <v>8</v>
@@ -39362,7 +39365,7 @@
         <v>445</v>
       </c>
       <c r="W443" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X443" s="16">
         <v>8</v>
@@ -39675,7 +39678,7 @@
         <v>445</v>
       </c>
       <c r="W448" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X448" s="16">
         <v>8</v>
@@ -39814,7 +39817,7 @@
         <v>445</v>
       </c>
       <c r="W450" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X450" s="16">
         <v>8</v>
@@ -39882,7 +39885,7 @@
         <v>445</v>
       </c>
       <c r="W451" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X451" s="16">
         <v>8</v>
@@ -40195,7 +40198,7 @@
         <v>445</v>
       </c>
       <c r="W456" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X456" s="16">
         <v>8</v>
@@ -40334,7 +40337,7 @@
         <v>445</v>
       </c>
       <c r="W458" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X458" s="16">
         <v>8</v>
@@ -40402,7 +40405,7 @@
         <v>445</v>
       </c>
       <c r="W459" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X459" s="16">
         <v>8</v>
@@ -40715,7 +40718,7 @@
         <v>445</v>
       </c>
       <c r="W464" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X464" s="16">
         <v>8</v>
@@ -40789,7 +40792,7 @@
         <v>445</v>
       </c>
       <c r="W465" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X465" s="16">
         <v>8</v>
@@ -40857,7 +40860,7 @@
         <v>445</v>
       </c>
       <c r="W466" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X466" s="16">
         <v>8</v>
@@ -41105,7 +41108,7 @@
         <v>445</v>
       </c>
       <c r="W470" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X470" s="16">
         <v>8</v>
@@ -41179,7 +41182,7 @@
         <v>445</v>
       </c>
       <c r="W471" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X471" s="16">
         <v>8</v>
@@ -41247,7 +41250,7 @@
         <v>445</v>
       </c>
       <c r="W472" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X472" s="16">
         <v>8</v>

</xml_diff>